<commit_message>
adicionei os requesitos novos no excel
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Uni\3rd Year\2 Semester\Base de dados\trabalho_bd\tpbasesdados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0DCB6E-4ADD-44BD-8881-38CBD6CA2714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{032F0202-B7F4-432F-A4A6-C4F8DBB19462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definição" sheetId="4" r:id="rId1"/>
@@ -1079,7 +1079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9951260F-6E12-4ADE-A61C-386784AA1F72}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="84" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="84" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -2550,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
retifiquei as definições das entidades do excel
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{032F0202-B7F4-432F-A4A6-C4F8DBB19462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898950A-BF46-4F68-A9C6-3890FBBD8EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,28 +252,7 @@
     <t>Requisitos</t>
   </si>
   <si>
-    <t>Descrição detalhada de uma unidade do SNS do setor privado ou público responsável pela prestação de cuidados de saúde à população.</t>
-  </si>
-  <si>
     <t>A gestão de meios operacionais nomeadamente ambulâncias e outros veículos de socorro de urgência, é de grande relevância para a área da saúde uma vez que um pequeno erro pode custar uma vida. Quer seja este erro a má atribuição do veículo à missão, quer seja um equipamento não funcional. Um sistema de base de dados bem implementado torna-se então crucial para o bom funcionamento dos serviços de socorro a emergências disponibilizado pelas ULS. Nesta base de dados terão que ter sido em conta variados requisitos:</t>
-  </si>
-  <si>
-    <t>Caracterização detalhada de um meio de transporte que auxilia a prestação de cuidados de saúde à população e pertence a uma EPCS.</t>
-  </si>
-  <si>
-    <t>Caracterização de indivíduos que receberam de cuidados médicos numa determinada EPCS.</t>
-  </si>
-  <si>
-    <t>Descrição geral de uma ULS, isto é, de um conjunto de EPCS que prestam, em conjunto, diferentes tipos de cuidados de saúde de uma determinada área geográfica e que constituem um grupo.</t>
-  </si>
-  <si>
-    <t>Caracterização detalhada de uma ferramenta essencial à prestação de cuidados de saúde à população, presente numa viatura de emergência.</t>
-  </si>
-  <si>
-    <t>Termo geral que descreve todos os especialistas médicos que empregam uma determinada missão para prestar cuidados de saúde à população.</t>
-  </si>
-  <si>
-    <t>Descrição geral de um ato, com o objetivo de proporcionar cuidados de saúde de qualidade à população, assegurando uma resposta rápida e eficiente em situações de emergência.</t>
   </si>
   <si>
     <t>TINYINT</t>
@@ -345,6 +324,27 @@
   <si>
     <t>Deve ser possível identificar os EPCS pelo nif, nome, morada, código postal, localidade, número de registo, contacto e endereço de email, 
 e a ULS a que pertencem.</t>
+  </si>
+  <si>
+    <t>Entidade que agrupo os ECPS e ela mesma está agrupada por grupos</t>
+  </si>
+  <si>
+    <t>Viatura afeta a uma EPCS, utilizada em missões, podendo transportar equipamentos e profissionais.</t>
+  </si>
+  <si>
+    <t>Representa as ECPS, à qual pertencem as viaturas, opera no âmbito de uma ULS</t>
+  </si>
+  <si>
+    <t>Equipamento transportado em viaturas, detalhado rigorasamente, sujeito a inspeções periódicas.</t>
+  </si>
+  <si>
+    <t>Termo geral que define uma peesoa qualificada a prestar cuidados de saúde, podendo estar associada a missões.</t>
+  </si>
+  <si>
+    <t>Atividade operacional que envolve uma viatura, profissionais e eventualmente pacientes.</t>
+  </si>
+  <si>
+    <t>Pessoa que recebe cuidados de saúde. Pode ser identificada de forma parcial em emergências.</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1093,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
@@ -1240,7 +1240,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C12" s="37"/>
       <c r="D12" s="37"/>
@@ -1284,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="37"/>
@@ -1392,7 +1392,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C19" s="37"/>
       <c r="D19" s="37"/>
@@ -1436,7 +1436,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C21" s="37"/>
       <c r="D21" s="37"/>
@@ -1480,7 +1480,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="37"/>
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C25" s="37"/>
       <c r="D25" s="37"/>
@@ -1568,7 +1568,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="37"/>
@@ -1612,7 +1612,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
@@ -1656,7 +1656,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C31" s="37"/>
       <c r="D31" s="37"/>
@@ -1700,7 +1700,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="37"/>
@@ -1744,7 +1744,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C35" s="37"/>
       <c r="D35" s="37"/>
@@ -1788,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C37" s="37"/>
       <c r="D37" s="37"/>
@@ -1832,7 +1832,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C39" s="37"/>
       <c r="D39" s="37"/>
@@ -1876,7 +1876,7 @@
         <v>15</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="37"/>
@@ -1920,7 +1920,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="37"/>
@@ -2551,7 +2551,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2568,12 +2568,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2581,7 +2581,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2589,7 +2589,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2597,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2605,15 +2605,15 @@
         <v>7</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2621,7 +2621,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3133,7 +3133,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>41</v>
@@ -3186,7 +3186,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>42</v>
@@ -4247,7 +4247,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
@@ -4256,7 +4256,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -4264,16 +4264,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
requisito 3, data de fabrico -> data de primeira matrícula  (linguagem legal) requisito 7, "participaram da missão" -> "participaram numa dada missão" requisito 8, "codigo" -> "código" requisito 10, "codigo" -> "código" requisito 13, adicionado "No caso de não ser encontrada correspondência, tal deve ser indicado." requisito 15, "engariar" -> "angariar" requisito 16, "inserior" -> "inserir" requisito 16, "sem este estar associado a alguma entidade já" -> "assegurando que o telefone ainda não se encontra associado a algum registo"
rewording do requisito 10

diagramaER:
-viatura/data_inspecao_proxima para atributo derivado (depende de data matricula e data inspeção anterior)
-similar para o equipamento

"assistencia" -> "assistência" tanto nos relacionamentos do excel como no ER
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\um_no\Desktop\bases dados\00 backups\3 sabado meio da tarde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898950A-BF46-4F68-A9C6-3890FBBD8EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BB8E61-C02D-4685-9171-0A97A2316711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definição" sheetId="4" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t xml:space="preserve">Missao </t>
   </si>
   <si>
-    <t>assistencia</t>
-  </si>
-  <si>
     <t>1...*</t>
   </si>
   <si>
@@ -276,18 +273,12 @@
     <t>Deve ser possível identificar as ULS pelo seu nome e grupo.</t>
   </si>
   <si>
-    <t>Uma viatura deve ser identificável pela sua matrícula, tipologia, data de fabrico, marca, data de inspeção anterior e próxima.</t>
-  </si>
-  <si>
     <t>Deve ser possível conseguir identificar a que EPCS pertence uma viatura, assim como se se encontra de momento em missão ou não.</t>
   </si>
   <si>
     <t>Uma missão deve ser identificada por descrição, tipo de missão, data e hora de ínicio e fim da mesma, assim como que viatura foi utilizada.</t>
   </si>
   <si>
-    <t>Deve ser possível consultar quais os profissionais de saúde participaram da missão assim como que pacientes foram atendidos.</t>
-  </si>
-  <si>
     <t>Também deve ser possível verificar se um profissional se encontra ativo em missão no momento.</t>
   </si>
   <si>
@@ -297,31 +288,13 @@
     <t>Não deve ser possível criar uma nova missão com uma viatura que se encontra com a inspeção desatualizada.</t>
   </si>
   <si>
-    <t>Deve ser possível identificar a entidade a qual pertence um NIF.</t>
-  </si>
-  <si>
     <t>O formato dos emails inseridos deve ser válido, seguindo uma estrutura genérica de emails.</t>
-  </si>
-  <si>
-    <t>Deve ser possível criar ou atualizar novos pacientes, com a informação possível de engariar pelos profissionais durante a missão.</t>
   </si>
   <si>
     <t>Os equipamentos presentes numa viatura devem ser identificáveis pelo seu número de série, descrição, quantidade, data de inspeção anterior e proxima,
 e um tipo, com um intervalo de inspeção especificado.</t>
   </si>
   <si>
-    <t>Deve ser possível identificar o nif, cédula profissional, cc, nome, morada, data de nascimento, telefone, descrição, 
-categoria e codigo postal associado a uma localidade de um profissional.</t>
-  </si>
-  <si>
-    <t>Deve ser possível identificar os pacientes mesmo se estes não forem capazes de se identificarem no cenário de emergência, mas se conseguirem terão de poder ser 
-identificados por nome, cc, nif, morada, data de nascimento, codigo postal e telefone do mesmo.</t>
-  </si>
-  <si>
-    <t>Deve ser possível inserior o número de telefone de uma entidade existente com base no respetivo NIF, sem este estar associado a alguma entidade já, e cumprindo o formato
-tradicional de número telefónicos em Portugal.</t>
-  </si>
-  <si>
     <t>Deve ser possível identificar os EPCS pelo nif, nome, morada, código postal, localidade, número de registo, contacto e endereço de email, 
 e a ULS a que pertencem.</t>
   </si>
@@ -338,13 +311,39 @@
     <t>Equipamento transportado em viaturas, detalhado rigorasamente, sujeito a inspeções periódicas.</t>
   </si>
   <si>
-    <t>Termo geral que define uma peesoa qualificada a prestar cuidados de saúde, podendo estar associada a missões.</t>
-  </si>
-  <si>
     <t>Atividade operacional que envolve uma viatura, profissionais e eventualmente pacientes.</t>
   </si>
   <si>
     <t>Pessoa que recebe cuidados de saúde. Pode ser identificada de forma parcial em emergências.</t>
+  </si>
+  <si>
+    <t>Uma viatura deve ser identificável pela sua matrícula, tipologia, data de primeira matrícula, marca, data de inspeção anterior e próxima.</t>
+  </si>
+  <si>
+    <t>Deve ser possível identificar o nif, cédula profissional, cc, nome, morada, data de nascimento, telefone, descrição, 
+categoria e código postal associado a uma localidade de um profissional.</t>
+  </si>
+  <si>
+    <t>Deve ser possível identificar a entidade a qual pertence um NIF. No caso de não ser encontrada correspondência, tal deve ser indicado.</t>
+  </si>
+  <si>
+    <t>Deve ser possível inserir o número de telefone de uma entidade existente com base no respetivo NIF, assegurando que o telefone ainda não se encontra associado a algum registo, e cumprindo o formato
+tradicional de número telefónicos em Portugal.</t>
+  </si>
+  <si>
+    <t>Deve ser possível criar ou atualizar novos pacientes, com a informação possível de angariar pelos profissionais durante a missão.</t>
+  </si>
+  <si>
+    <t>Deve ser possível consultar quais os profissionais de saúde participaram  numa dada missão, assim como que pacientes foram atendidos.</t>
+  </si>
+  <si>
+    <t>Deve ser possível a identificação dos pacientes, ainda que não seja possível a determinar todas as informações no cenário de emergência: os profissionais devem conseguir recolher o máximo de elementos identificativos dos pacientes, nomeadamente nome, cc, nif, morada, data de nascimento, código postal e número de telefone, sendo possível colocar valores nulos nestes campos.</t>
+  </si>
+  <si>
+    <t>assistência</t>
+  </si>
+  <si>
+    <t>Termo geral que define uma pessoa qualificada a prestar cuidados de saúde, podendo estar associada a missões.</t>
   </si>
 </sst>
 </file>
@@ -620,7 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -712,6 +711,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -724,18 +726,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -748,6 +747,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,12 +791,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1079,129 +1075,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9951260F-6E12-4ADE-A61C-386784AA1F72}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="84" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="A30" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:R50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="8.88671875" style="2"/>
-    <col min="18" max="18" width="37.77734375" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="17" width="8.85546875" style="2"/>
+    <col min="18" max="18" width="37.7109375" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="43"/>
-    </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -1213,9 +1209,9 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
@@ -1235,1249 +1231,1249 @@
       <c r="Q11" s="46"/>
       <c r="R11" s="47"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="41">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="43">
         <v>1</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="39"/>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="44"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="41"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
+        <v>2</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="39"/>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="44"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="41"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="43">
+        <v>3</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="39"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="48"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="42"/>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="41"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="43">
+        <v>4</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="39"/>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="44"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="41"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
+        <v>5</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="39"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="44"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="41"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="43">
+        <v>6</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="39"/>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="44"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="41"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="43">
+        <v>7</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="39"/>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="44"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="41"/>
+    </row>
+    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="43">
+        <v>8</v>
+      </c>
+      <c r="B27" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37"/>
-      <c r="O12" s="37"/>
-      <c r="P12" s="37"/>
-      <c r="Q12" s="37"/>
-      <c r="R12" s="38"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="42"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="40"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="41">
-        <v>2</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="38"/>
-    </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="42"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="40"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="41">
-        <v>3</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="38"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="44"/>
-    </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="42"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="40"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="41">
-        <v>4</v>
-      </c>
-      <c r="B19" s="37" t="s">
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="39"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="44"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="41"/>
+    </row>
+    <row r="29" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43">
+        <v>9</v>
+      </c>
+      <c r="B29" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="38"/>
-    </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="42"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="40"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="41">
-        <v>5</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="38"/>
-    </row>
-    <row r="22" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="42"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="40"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="41">
-        <v>6</v>
-      </c>
-      <c r="B23" s="37" t="s">
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="39"/>
+    </row>
+    <row r="30" spans="1:18" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="44"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="41"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="43">
+        <v>10</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="39"/>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="44"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="41"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="43">
+        <v>11</v>
+      </c>
+      <c r="B33" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="37"/>
-      <c r="R23" s="38"/>
-    </row>
-    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="42"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
-      <c r="R24" s="40"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="41">
-        <v>7</v>
-      </c>
-      <c r="B25" s="37" t="s">
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="39"/>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="44"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="41"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="43">
+        <v>12</v>
+      </c>
+      <c r="B35" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="38"/>
-    </row>
-    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="42"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="40"/>
-    </row>
-    <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="41">
-        <v>8</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="38"/>
-    </row>
-    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="42"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="40"/>
-    </row>
-    <row r="29" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="41">
-        <v>9</v>
-      </c>
-      <c r="B29" s="37" t="s">
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="39"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="44"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="41"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="43">
+        <v>13</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="39"/>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="44"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="40"/>
+      <c r="R38" s="41"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="43">
+        <v>14</v>
+      </c>
+      <c r="B39" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="38"/>
-    </row>
-    <row r="30" spans="1:18" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="42"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="40"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="41">
-        <v>10</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="38"/>
-    </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="42"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="40"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="41">
-        <v>11</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="38"/>
-    </row>
-    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="42"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="40"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="41">
-        <v>12</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="37"/>
-      <c r="Q35" s="37"/>
-      <c r="R35" s="38"/>
-    </row>
-    <row r="36" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="42"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="40"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="41">
-        <v>13</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-      <c r="L37" s="37"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="37"/>
-      <c r="P37" s="37"/>
-      <c r="Q37" s="37"/>
-      <c r="R37" s="38"/>
-    </row>
-    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="42"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="39"/>
-      <c r="R38" s="40"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="41">
-        <v>14</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
-      <c r="P39" s="37"/>
-      <c r="Q39" s="37"/>
-      <c r="R39" s="38"/>
-    </row>
-    <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="42"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
-      <c r="N40" s="39"/>
-      <c r="O40" s="39"/>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="39"/>
-      <c r="R40" s="40"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="41">
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="39"/>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="44"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="40"/>
+      <c r="R40" s="41"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="43">
         <v>15</v>
       </c>
-      <c r="B41" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
-      <c r="K41" s="37"/>
-      <c r="L41" s="37"/>
-      <c r="M41" s="37"/>
-      <c r="N41" s="37"/>
-      <c r="O41" s="37"/>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="37"/>
-      <c r="R41" s="38"/>
-    </row>
-    <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="42"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="39"/>
-      <c r="R42" s="40"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="41">
+      <c r="B41" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="39"/>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="44"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="40"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="40"/>
+      <c r="Q42" s="40"/>
+      <c r="R42" s="41"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="43">
         <v>16</v>
       </c>
-      <c r="B43" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="37"/>
-      <c r="M43" s="37"/>
-      <c r="N43" s="37"/>
-      <c r="O43" s="37"/>
-      <c r="P43" s="37"/>
-      <c r="Q43" s="37"/>
-      <c r="R43" s="38"/>
-    </row>
-    <row r="44" spans="1:18" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="42"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
-      <c r="R44" s="40"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="64"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="63"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="63"/>
-      <c r="R45" s="63"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="64"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
-      <c r="K46" s="63"/>
-      <c r="L46" s="63"/>
-      <c r="M46" s="63"/>
-      <c r="N46" s="63"/>
-      <c r="O46" s="63"/>
-      <c r="P46" s="63"/>
-      <c r="Q46" s="63"/>
-      <c r="R46" s="63"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="64"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="63"/>
-      <c r="P47" s="63"/>
-      <c r="Q47" s="63"/>
-      <c r="R47" s="63"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="64"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="63"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="63"/>
-      <c r="F48" s="63"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="63"/>
-      <c r="I48" s="63"/>
-      <c r="J48" s="63"/>
-      <c r="K48" s="63"/>
-      <c r="L48" s="63"/>
-      <c r="M48" s="63"/>
-      <c r="N48" s="63"/>
-      <c r="O48" s="63"/>
-      <c r="P48" s="63"/>
-      <c r="Q48" s="63"/>
-      <c r="R48" s="63"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A49" s="64"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="63"/>
-      <c r="K49" s="63"/>
-      <c r="L49" s="63"/>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-      <c r="O49" s="63"/>
-      <c r="P49" s="63"/>
-      <c r="Q49" s="63"/>
-      <c r="R49" s="63"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A50" s="64"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="63"/>
-      <c r="J50" s="63"/>
-      <c r="K50" s="63"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-      <c r="O50" s="63"/>
-      <c r="P50" s="63"/>
-      <c r="Q50" s="63"/>
-      <c r="R50" s="63"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="64"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="63"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="63"/>
-      <c r="J51" s="63"/>
-      <c r="K51" s="63"/>
-      <c r="L51" s="63"/>
-      <c r="M51" s="63"/>
-      <c r="N51" s="63"/>
-      <c r="O51" s="63"/>
-      <c r="P51" s="63"/>
-      <c r="Q51" s="63"/>
-      <c r="R51" s="63"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="64"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="63"/>
-      <c r="H52" s="63"/>
-      <c r="I52" s="63"/>
-      <c r="J52" s="63"/>
-      <c r="K52" s="63"/>
-      <c r="L52" s="63"/>
-      <c r="M52" s="63"/>
-      <c r="N52" s="63"/>
-      <c r="O52" s="63"/>
-      <c r="P52" s="63"/>
-      <c r="Q52" s="63"/>
-      <c r="R52" s="63"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A53" s="64"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="63"/>
-      <c r="G53" s="63"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="63"/>
-      <c r="J53" s="63"/>
-      <c r="K53" s="63"/>
-      <c r="L53" s="63"/>
-      <c r="M53" s="63"/>
-      <c r="N53" s="63"/>
-      <c r="O53" s="63"/>
-      <c r="P53" s="63"/>
-      <c r="Q53" s="63"/>
-      <c r="R53" s="63"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="64"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="63"/>
-      <c r="D54" s="63"/>
-      <c r="E54" s="63"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="63"/>
-      <c r="H54" s="63"/>
-      <c r="I54" s="63"/>
-      <c r="J54" s="63"/>
-      <c r="K54" s="63"/>
-      <c r="L54" s="63"/>
-      <c r="M54" s="63"/>
-      <c r="N54" s="63"/>
-      <c r="O54" s="63"/>
-      <c r="P54" s="63"/>
-      <c r="Q54" s="63"/>
-      <c r="R54" s="63"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A55" s="64"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="63"/>
-      <c r="G55" s="63"/>
-      <c r="H55" s="63"/>
-      <c r="I55" s="63"/>
-      <c r="J55" s="63"/>
-      <c r="K55" s="63"/>
-      <c r="L55" s="63"/>
-      <c r="M55" s="63"/>
-      <c r="N55" s="63"/>
-      <c r="O55" s="63"/>
-      <c r="P55" s="63"/>
-      <c r="Q55" s="63"/>
-      <c r="R55" s="63"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A56" s="64"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="63"/>
-      <c r="D56" s="63"/>
-      <c r="E56" s="63"/>
-      <c r="F56" s="63"/>
-      <c r="G56" s="63"/>
-      <c r="H56" s="63"/>
-      <c r="I56" s="63"/>
-      <c r="J56" s="63"/>
-      <c r="K56" s="63"/>
-      <c r="L56" s="63"/>
-      <c r="M56" s="63"/>
-      <c r="N56" s="63"/>
-      <c r="O56" s="63"/>
-      <c r="P56" s="63"/>
-      <c r="Q56" s="63"/>
-      <c r="R56" s="63"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A57" s="64"/>
-      <c r="B57" s="63"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
-      <c r="I57" s="63"/>
-      <c r="J57" s="63"/>
-      <c r="K57" s="63"/>
-      <c r="L57" s="63"/>
-      <c r="M57" s="63"/>
-      <c r="N57" s="63"/>
-      <c r="O57" s="63"/>
-      <c r="P57" s="63"/>
-      <c r="Q57" s="63"/>
-      <c r="R57" s="63"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A58" s="64"/>
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
-      <c r="E58" s="63"/>
-      <c r="F58" s="63"/>
-      <c r="G58" s="63"/>
-      <c r="H58" s="63"/>
-      <c r="I58" s="63"/>
-      <c r="J58" s="63"/>
-      <c r="K58" s="63"/>
-      <c r="L58" s="63"/>
-      <c r="M58" s="63"/>
-      <c r="N58" s="63"/>
-      <c r="O58" s="63"/>
-      <c r="P58" s="63"/>
-      <c r="Q58" s="63"/>
-      <c r="R58" s="63"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A59" s="64"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="63"/>
-      <c r="D59" s="63"/>
-      <c r="E59" s="63"/>
-      <c r="F59" s="63"/>
-      <c r="G59" s="63"/>
-      <c r="H59" s="63"/>
-      <c r="I59" s="63"/>
-      <c r="J59" s="63"/>
-      <c r="K59" s="63"/>
-      <c r="L59" s="63"/>
-      <c r="M59" s="63"/>
-      <c r="N59" s="63"/>
-      <c r="O59" s="63"/>
-      <c r="P59" s="63"/>
-      <c r="Q59" s="63"/>
-      <c r="R59" s="63"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A60" s="64"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="63"/>
-      <c r="D60" s="63"/>
-      <c r="E60" s="63"/>
-      <c r="F60" s="63"/>
-      <c r="G60" s="63"/>
-      <c r="H60" s="63"/>
-      <c r="I60" s="63"/>
-      <c r="J60" s="63"/>
-      <c r="K60" s="63"/>
-      <c r="L60" s="63"/>
-      <c r="M60" s="63"/>
-      <c r="N60" s="63"/>
-      <c r="O60" s="63"/>
-      <c r="P60" s="63"/>
-      <c r="Q60" s="63"/>
-      <c r="R60" s="63"/>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A61" s="64"/>
-      <c r="B61" s="63"/>
-      <c r="C61" s="63"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
-      <c r="F61" s="63"/>
-      <c r="G61" s="63"/>
-      <c r="H61" s="63"/>
-      <c r="I61" s="63"/>
-      <c r="J61" s="63"/>
-      <c r="K61" s="63"/>
-      <c r="L61" s="63"/>
-      <c r="M61" s="63"/>
-      <c r="N61" s="63"/>
-      <c r="O61" s="63"/>
-      <c r="P61" s="63"/>
-      <c r="Q61" s="63"/>
-      <c r="R61" s="63"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A62" s="64"/>
-      <c r="B62" s="63"/>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
-      <c r="I62" s="63"/>
-      <c r="J62" s="63"/>
-      <c r="K62" s="63"/>
-      <c r="L62" s="63"/>
-      <c r="M62" s="63"/>
-      <c r="N62" s="63"/>
-      <c r="O62" s="63"/>
-      <c r="P62" s="63"/>
-      <c r="Q62" s="63"/>
-      <c r="R62" s="63"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A63" s="64"/>
-      <c r="B63" s="63"/>
-      <c r="C63" s="63"/>
-      <c r="D63" s="63"/>
-      <c r="E63" s="63"/>
-      <c r="F63" s="63"/>
-      <c r="G63" s="63"/>
-      <c r="H63" s="63"/>
-      <c r="I63" s="63"/>
-      <c r="J63" s="63"/>
-      <c r="K63" s="63"/>
-      <c r="L63" s="63"/>
-      <c r="M63" s="63"/>
-      <c r="N63" s="63"/>
-      <c r="O63" s="63"/>
-      <c r="P63" s="63"/>
-      <c r="Q63" s="63"/>
-      <c r="R63" s="63"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A64" s="64"/>
-      <c r="B64" s="63"/>
-      <c r="C64" s="63"/>
-      <c r="D64" s="63"/>
-      <c r="E64" s="63"/>
-      <c r="F64" s="63"/>
-      <c r="G64" s="63"/>
-      <c r="H64" s="63"/>
-      <c r="I64" s="63"/>
-      <c r="J64" s="63"/>
-      <c r="K64" s="63"/>
-      <c r="L64" s="63"/>
-      <c r="M64" s="63"/>
-      <c r="N64" s="63"/>
-      <c r="O64" s="63"/>
-      <c r="P64" s="63"/>
-      <c r="Q64" s="63"/>
-      <c r="R64" s="63"/>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A65" s="64"/>
-      <c r="B65" s="63"/>
-      <c r="C65" s="63"/>
-      <c r="D65" s="63"/>
-      <c r="E65" s="63"/>
-      <c r="F65" s="63"/>
-      <c r="G65" s="63"/>
-      <c r="H65" s="63"/>
-      <c r="I65" s="63"/>
-      <c r="J65" s="63"/>
-      <c r="K65" s="63"/>
-      <c r="L65" s="63"/>
-      <c r="M65" s="63"/>
-      <c r="N65" s="63"/>
-      <c r="O65" s="63"/>
-      <c r="P65" s="63"/>
-      <c r="Q65" s="63"/>
-      <c r="R65" s="63"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A66" s="64"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="63"/>
-      <c r="D66" s="63"/>
-      <c r="E66" s="63"/>
-      <c r="F66" s="63"/>
-      <c r="G66" s="63"/>
-      <c r="H66" s="63"/>
-      <c r="I66" s="63"/>
-      <c r="J66" s="63"/>
-      <c r="K66" s="63"/>
-      <c r="L66" s="63"/>
-      <c r="M66" s="63"/>
-      <c r="N66" s="63"/>
-      <c r="O66" s="63"/>
-      <c r="P66" s="63"/>
-      <c r="Q66" s="63"/>
-      <c r="R66" s="63"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A67" s="64"/>
-      <c r="B67" s="63"/>
-      <c r="C67" s="63"/>
-      <c r="D67" s="63"/>
-      <c r="E67" s="63"/>
-      <c r="F67" s="63"/>
-      <c r="G67" s="63"/>
-      <c r="H67" s="63"/>
-      <c r="I67" s="63"/>
-      <c r="J67" s="63"/>
-      <c r="K67" s="63"/>
-      <c r="L67" s="63"/>
-      <c r="M67" s="63"/>
-      <c r="N67" s="63"/>
-      <c r="O67" s="63"/>
-      <c r="P67" s="63"/>
-      <c r="Q67" s="63"/>
-      <c r="R67" s="63"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A68" s="64"/>
-      <c r="B68" s="63"/>
-      <c r="C68" s="63"/>
-      <c r="D68" s="63"/>
-      <c r="E68" s="63"/>
-      <c r="F68" s="63"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="63"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="63"/>
-      <c r="K68" s="63"/>
-      <c r="L68" s="63"/>
-      <c r="M68" s="63"/>
-      <c r="N68" s="63"/>
-      <c r="O68" s="63"/>
-      <c r="P68" s="63"/>
-      <c r="Q68" s="63"/>
-      <c r="R68" s="63"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A69" s="64"/>
-      <c r="B69" s="63"/>
-      <c r="C69" s="63"/>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
-      <c r="F69" s="63"/>
-      <c r="G69" s="63"/>
-      <c r="H69" s="63"/>
-      <c r="I69" s="63"/>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="63"/>
-      <c r="M69" s="63"/>
-      <c r="N69" s="63"/>
-      <c r="O69" s="63"/>
-      <c r="P69" s="63"/>
-      <c r="Q69" s="63"/>
-      <c r="R69" s="63"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A70" s="64"/>
-      <c r="B70" s="63"/>
-      <c r="C70" s="63"/>
-      <c r="D70" s="63"/>
-      <c r="E70" s="63"/>
-      <c r="F70" s="63"/>
-      <c r="G70" s="63"/>
-      <c r="H70" s="63"/>
-      <c r="I70" s="63"/>
-      <c r="J70" s="63"/>
-      <c r="K70" s="63"/>
-      <c r="L70" s="63"/>
-      <c r="M70" s="63"/>
-      <c r="N70" s="63"/>
-      <c r="O70" s="63"/>
-      <c r="P70" s="63"/>
-      <c r="Q70" s="63"/>
-      <c r="R70" s="63"/>
+      <c r="B43" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="39"/>
+    </row>
+    <row r="44" spans="1:18" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="44"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="40"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="40"/>
+      <c r="R44" s="41"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45" s="49"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="49"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47" s="49"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="49"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="49"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="49"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="49"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="37"/>
+      <c r="P52" s="37"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="37"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="49"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="49"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="37"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="49"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="49"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
+      <c r="O56" s="37"/>
+      <c r="P56" s="37"/>
+      <c r="Q56" s="37"/>
+      <c r="R56" s="37"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57" s="49"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="37"/>
+      <c r="O57" s="37"/>
+      <c r="P57" s="37"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="49"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="37"/>
+      <c r="O58" s="37"/>
+      <c r="P58" s="37"/>
+      <c r="Q58" s="37"/>
+      <c r="R58" s="37"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="49"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="37"/>
+      <c r="O59" s="37"/>
+      <c r="P59" s="37"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="49"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="37"/>
+      <c r="O60" s="37"/>
+      <c r="P60" s="37"/>
+      <c r="Q60" s="37"/>
+      <c r="R60" s="37"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="49"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="37"/>
+      <c r="O61" s="37"/>
+      <c r="P61" s="37"/>
+      <c r="Q61" s="37"/>
+      <c r="R61" s="37"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="49"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="37"/>
+      <c r="O62" s="37"/>
+      <c r="P62" s="37"/>
+      <c r="Q62" s="37"/>
+      <c r="R62" s="37"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="49"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" s="37"/>
+      <c r="P63" s="37"/>
+      <c r="Q63" s="37"/>
+      <c r="R63" s="37"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" s="49"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" s="37"/>
+      <c r="P64" s="37"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="37"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="49"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="37"/>
+      <c r="P65" s="37"/>
+      <c r="Q65" s="37"/>
+      <c r="R65" s="37"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A66" s="49"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+      <c r="L66" s="37"/>
+      <c r="M66" s="37"/>
+      <c r="N66" s="37"/>
+      <c r="O66" s="37"/>
+      <c r="P66" s="37"/>
+      <c r="Q66" s="37"/>
+      <c r="R66" s="37"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A67" s="49"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="37"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="37"/>
+      <c r="Q67" s="37"/>
+      <c r="R67" s="37"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="49"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A69" s="49"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="37"/>
+      <c r="O69" s="37"/>
+      <c r="P69" s="37"/>
+      <c r="Q69" s="37"/>
+      <c r="R69" s="37"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A70" s="49"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="37"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="37"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="37"/>
+      <c r="O70" s="37"/>
+      <c r="P70" s="37"/>
+      <c r="Q70" s="37"/>
+      <c r="R70" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="60">
@@ -2519,28 +2515,28 @@
     <mergeCell ref="B35:R36"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:R38"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:R24"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="B31:R32"/>
     <mergeCell ref="B29:R30"/>
     <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:R28"/>
     <mergeCell ref="B1:K9"/>
     <mergeCell ref="B12:R13"/>
     <mergeCell ref="B14:R15"/>
     <mergeCell ref="B16:R18"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:R26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:R28"/>
     <mergeCell ref="A11:R11"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:R20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:R22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:R24"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2551,16 +2547,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="134.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2568,60 +2564,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2633,64 +2629,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445FE2A4-4568-4C19-AD65-4FDDB4A8E56D}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L82" sqref="L82"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="7" width="14.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="2"/>
+    <col min="6" max="7" width="14.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="2" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="47.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:9" ht="47.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="56" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="60"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="56"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="61"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="57"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2718,13 +2714,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>41</v>
@@ -2745,13 +2741,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="51"/>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
       <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>41</v>
@@ -2772,8 +2768,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="49" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -2801,13 +2797,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
       <c r="B7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>41</v>
@@ -2828,13 +2824,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
       <c r="B8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>41</v>
@@ -2855,13 +2851,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>41</v>
@@ -2882,13 +2878,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>41</v>
@@ -2909,8 +2905,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2936,8 +2932,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
@@ -2963,13 +2959,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="51"/>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="52"/>
       <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>41</v>
@@ -2990,15 +2986,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="50" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>40</v>
@@ -3019,10 +3015,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
@@ -3046,13 +3042,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>41</v>
@@ -3073,13 +3069,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
       <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>41</v>
@@ -3100,8 +3096,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
       <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
@@ -3127,13 +3123,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
       <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>41</v>
@@ -3154,8 +3150,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="51"/>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
       <c r="B20" s="10" t="s">
         <v>31</v>
       </c>
@@ -3181,12 +3177,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="49" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>42</v>
@@ -3210,13 +3206,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
       <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>41</v>
@@ -3237,13 +3233,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>41</v>
@@ -3264,13 +3260,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="50"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>41</v>
@@ -3291,13 +3287,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="50"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="51"/>
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>41</v>
@@ -3318,10 +3314,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="51"/>
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>42</v>
@@ -3345,8 +3341,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="51"/>
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
@@ -3372,8 +3368,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="50"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="51"/>
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
@@ -3399,8 +3395,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="51"/>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="52"/>
       <c r="B29" s="10" t="s">
         <v>31</v>
       </c>
@@ -3426,8 +3422,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="49" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -3455,8 +3451,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="50"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
       <c r="B31" s="2" t="s">
         <v>35</v>
       </c>
@@ -3482,8 +3478,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="50"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="51"/>
       <c r="B32" s="2" t="s">
         <v>36</v>
       </c>
@@ -3509,13 +3505,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="50"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="51"/>
       <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>41</v>
@@ -3536,8 +3532,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="50"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="51"/>
       <c r="B34" s="2" t="s">
         <v>37</v>
       </c>
@@ -3563,13 +3559,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="50"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="51"/>
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>41</v>
@@ -3590,13 +3586,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="50"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="51"/>
       <c r="B36" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>41</v>
@@ -3617,13 +3613,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="50"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="51"/>
       <c r="B37" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>41</v>
@@ -3644,8 +3640,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="50"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="51"/>
       <c r="B38" s="2" t="s">
         <v>24</v>
       </c>
@@ -3671,13 +3667,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="51"/>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="52"/>
       <c r="B39" s="10" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>41</v>
@@ -3698,8 +3694,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="52" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="53" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="30" t="s">
@@ -3727,13 +3723,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="53"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="54"/>
       <c r="B41" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>41</v>
@@ -3754,13 +3750,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="53"/>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="54"/>
       <c r="B42" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>41</v>
@@ -3781,13 +3777,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="53"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="54"/>
       <c r="B43" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>41</v>
@@ -3808,40 +3804,40 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="53"/>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="54"/>
       <c r="B44" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="53"/>
-      <c r="B45" s="31" t="s">
+      <c r="C45" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>41</v>
@@ -3862,13 +3858,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="54"/>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="55"/>
       <c r="B46" s="32" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>41</v>
@@ -3889,8 +3885,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="49" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -3918,10 +3914,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="51"/>
       <c r="B48" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>42</v>
@@ -3945,8 +3941,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="50"/>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="51"/>
       <c r="B49" s="2" t="s">
         <v>19</v>
       </c>
@@ -3972,13 +3968,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="50"/>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="51"/>
       <c r="B50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>41</v>
@@ -3999,8 +3995,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="50"/>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="51"/>
       <c r="B51" s="2" t="s">
         <v>37</v>
       </c>
@@ -4026,13 +4022,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="50"/>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="51"/>
       <c r="B52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>41</v>
@@ -4053,13 +4049,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="50"/>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="51"/>
       <c r="B53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>41</v>
@@ -4080,13 +4076,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="50"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="51"/>
       <c r="B54" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>41</v>
@@ -4107,8 +4103,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="51"/>
+    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="52"/>
       <c r="B55" s="10" t="s">
         <v>24</v>
       </c>
@@ -4162,19 +4158,19 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
@@ -4191,12 +4187,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>49</v>
@@ -4205,15 +4201,15 @@
         <v>2</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>49</v>
@@ -4225,12 +4221,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
@@ -4242,12 +4238,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
         <v>51</v>
@@ -4256,27 +4252,27 @@
         <v>6</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>52</v>
       </c>
@@ -4284,16 +4280,16 @@
         <v>48</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="16"/>
       <c r="C18" s="15"/>

</xml_diff>